<commit_message>
did a bit more data wrangling, as there were some mistakes in the previous version. began very preliminary EDA
</commit_message>
<xml_diff>
--- a/Data/draftOrder09to19.xlsx
+++ b/Data/draftOrder09to19.xlsx
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A301" workbookViewId="0">
-      <selection activeCell="B335" sqref="B335"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="B256" sqref="B256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3309,7 +3309,7 @@
         <v>9</v>
       </c>
       <c r="B253" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C253">
         <v>2011</v>

</xml_diff>

<commit_message>
matched season n stats with season n + 1 performance, last bits of data cleaning, did a bit more EDA
</commit_message>
<xml_diff>
--- a/Data/draftOrder09to19.xlsx
+++ b/Data/draftOrder09to19.xlsx
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
-      <selection activeCell="B256" sqref="B256"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="D211" sqref="D211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2858,7 +2858,7 @@
         <v>28</v>
       </c>
       <c r="B212" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C212">
         <v>2013</v>

</xml_diff>